<commit_message>
[WIP] Add tests for Saliva Check-in validates against all missing fields
CVDLS-201
</commit_message>
<xml_diff>
--- a/tests/ExcelImport/workbooks/tube-checkin-saliva.xlsx
+++ b/tests/ExcelImport/workbooks/tube-checkin-saliva.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jok/Projects/covid-symfony-prototype/tests/ExcelImport/workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3924CE6D-5721-9747-A1AB-5845716D57B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A804CC62-8F45-CE4E-9762-D16A08BDCD7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="17540" xr2:uid="{D641F29D-EB73-5746-B974-A2176733CB0B}"/>
+    <workbookView xWindow="2620" yWindow="460" windowWidth="26180" windowHeight="17540" xr2:uid="{D641F29D-EB73-5746-B974-A2176733CB0B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="23">
   <si>
     <t>Tube ID</t>
   </si>
@@ -87,6 +87,21 @@
   </si>
   <si>
     <t>TestCheckin0007</t>
+  </si>
+  <si>
+    <t>Tests empty Accepted/Rejected (REQUIRED)</t>
+  </si>
+  <si>
+    <t>Tests empty Tube ID (REQUIRED)</t>
+  </si>
+  <si>
+    <t>Tests empty Well Plate Barcode (OPTIONAL)</t>
+  </si>
+  <si>
+    <t>Tests empty Kit Type (OPTIONAL)</t>
+  </si>
+  <si>
+    <t>Tests empty Username (REQUIRED)</t>
   </si>
 </sst>
 </file>
@@ -108,12 +123,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -128,8 +155,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{966E636C-4996-8A44-87BF-81C75963A000}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -458,7 +488,7 @@
     <col min="4" max="4" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -475,7 +505,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -492,7 +522,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -509,27 +539,29 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
+      <c r="B6" s="1"/>
       <c r="C6" t="s">
         <v>7</v>
       </c>
@@ -539,41 +571,44 @@
       <c r="E6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="2"/>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>17</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
@@ -581,11 +616,44 @@
       <c r="C9" t="s">
         <v>7</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="3"/>
+      <c r="E9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
         <v>8</v>
       </c>
-      <c r="E9" t="s">
-        <v>10</v>
+      <c r="E11" s="1"/>
+      <c r="F11" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TubeCheckinSalivaImporter validates against all required fields
And adds tests

CVDLS-201
</commit_message>
<xml_diff>
--- a/tests/ExcelImport/workbooks/tube-checkin-saliva.xlsx
+++ b/tests/ExcelImport/workbooks/tube-checkin-saliva.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jok/Projects/covid-symfony-prototype/tests/ExcelImport/workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A804CC62-8F45-CE4E-9762-D16A08BDCD7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{229E7088-F293-0243-BD5C-EF770A9CB450}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2620" yWindow="460" windowWidth="26180" windowHeight="17540" xr2:uid="{D641F29D-EB73-5746-B974-A2176733CB0B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="24">
   <si>
     <t>Tube ID</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>Tests empty Username (REQUIRED)</t>
+  </si>
+  <si>
+    <t>TestCheckin0008</t>
   </si>
 </sst>
 </file>
@@ -477,7 +480,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -577,7 +580,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -592,7 +595,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -608,7 +611,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
@@ -626,7 +629,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
@@ -640,7 +643,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>

</xml_diff>